<commit_message>
feat: explo ortho 2024 & dim_damir
</commit_message>
<xml_diff>
--- a/docs/2024_descriptif-variables_open-damir-base-complete.xlsx
+++ b/docs/2024_descriptif-variables_open-damir-base-complete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine.Giraud\Documents\code\damir_actes_secu\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0624223B-9B72-4F9E-B9CB-3845EF98F819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5CC42A-416C-4751-8053-69ECB49C9067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IR_PHA_R" sheetId="1" r:id="rId1"/>
@@ -10379,17 +10379,17 @@
     </r>
   </si>
   <si>
+    <t>valeur</t>
+  </si>
+  <si>
+    <t>Le coefficient global est préfiltré sur le type de remboursement (PRS_REM_TYP) 0, il contient déjà le coefficient global de tous les types de remboursement.
+NB : Si ce filtre n'est pas fait, les coefficients seront doublés.
+Il représente un volume : quantité x coefficient tarifé de l'acte.</t>
+  </si>
+  <si>
     <t>Indicateurs bruts destinés aux utilisateurs avertis des données, qui maitrisent les filtres sur les types de remboursement : 
 - filtre impératif sur type de remboursement = 0 pour  comptabiliser les prestations sans doublon de type de remboursement puisque la totalité du coefficient global se trouve au sein de la modalité 0
 - filtre sur un type de remboursement &lt;&gt; 0 (choisir la valeur de la modalité en fonction du type de remboursement précis).
-Il représente un volume : quantité x coefficient tarifé de l'acte.</t>
-  </si>
-  <si>
-    <t>valeur</t>
-  </si>
-  <si>
-    <t>Le coefficient global est préfiltré sur le type de remboursement (PRS_REM_TYP) 0, il contient déjà le coefficient global de tous les types de remboursement.
-NB : Si ce filtre n'est pas fait, les coefficients seront doublés.
 Il représente un volume : quantité x coefficient tarifé de l'acte.</t>
   </si>
 </sst>
@@ -10716,7 +10716,7 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10794,6 +10794,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -10815,28 +10836,6 @@
     <xf numFmtId="3" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
@@ -10845,10 +10844,7 @@
     <cellStyle name="Titre 1" xfId="1" builtinId="16"/>
     <cellStyle name="Titre 4" xfId="2" builtinId="19"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -10890,64 +10886,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -10999,19 +10938,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B86E43E-9D10-41B6-AEA0-A1C4F39F5AFB}" name="Tableau1" displayName="Tableau1" ref="A1:J12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B86E43E-9D10-41B6-AEA0-A1C4F39F5AFB}" name="Tableau1" displayName="Tableau1" ref="A1:J12" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:J12" xr:uid="{1B86E43E-9D10-41B6-AEA0-A1C4F39F5AFB}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E8471B5B-569B-4B11-B580-05E5ADA70D69}" name="nom_variable" dataDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{9CDB183F-001E-4801-878D-C3869B2F8DD1}" name="libelle_variable" dataDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{38DA90ED-1682-4EA3-9C85-E847C7A73C89}" name="Exemple fictif" dataDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{272EAF53-6967-4824-9924-FF435C67F31A}" name="concept_1" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{111E5C5B-9DF5-4645-9AD3-719D2DD41060}" name="concept_2" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{999F0405-AA18-40AF-9F2D-47332E7D5838}" name="concept_3" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{83ABA864-DE51-4869-801B-F1C1EF3F9951}" name="concept_4" dataDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{DBA5CB24-13FC-4E5F-916D-F2C1DB4C781A}" name="rdg_1" dataDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{913D5C38-403E-4C81-BBBF-5774421B6C2D}" name="observations" dataDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{D31EAEBD-1C74-4E5A-92C0-AFE4478FBEAB}" name="sensible_medical" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{E8471B5B-569B-4B11-B580-05E5ADA70D69}" name="nom_variable" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{9CDB183F-001E-4801-878D-C3869B2F8DD1}" name="libelle_variable" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{38DA90ED-1682-4EA3-9C85-E847C7A73C89}" name="Exemple fictif" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{272EAF53-6967-4824-9924-FF435C67F31A}" name="concept_1" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{111E5C5B-9DF5-4645-9AD3-719D2DD41060}" name="concept_2" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{999F0405-AA18-40AF-9F2D-47332E7D5838}" name="concept_3" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{83ABA864-DE51-4869-801B-F1C1EF3F9951}" name="concept_4" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{DBA5CB24-13FC-4E5F-916D-F2C1DB4C781A}" name="rdg_1" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{913D5C38-403E-4C81-BBBF-5774421B6C2D}" name="observations" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{D31EAEBD-1C74-4E5A-92C0-AFE4478FBEAB}" name="sensible_medical" dataDxfId="5" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11027,7 +10966,7 @@
     <tableColumn id="1" xr3:uid="{81561C7C-EB4E-4897-A1DB-3F9ABD6D7988}" name="Nom variable" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{F97B2A34-707C-40B2-AD00-3A7AB01319E3}" name="Libellé" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{3F9EEEE9-B5F4-4FF0-B2D5-825CF8907DD4}" name="Catégorie" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{EDCFD4B2-5585-46D8-AA35-7902C0B6A663}" name="Commentaires" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{EDCFD4B2-5585-46D8-AA35-7902C0B6A663}" name="Commentaires" dataDxfId="4" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{0705ED08-F953-411E-A984-44CEC3CCF088}" name="Modalités" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -11325,7 +11264,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -11345,326 +11284,326 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="28" t="s">
         <v>3382</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="28" t="s">
         <v>3383</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="28" t="s">
         <v>3384</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="28" t="s">
         <v>3385</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="28" t="s">
         <v>3386</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="28" t="s">
         <v>3387</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="28" t="s">
         <v>3388</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="28" t="s">
         <v>3389</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="28" t="s">
         <v>3390</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="28" t="s">
         <v>3391</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="22" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="28" t="s">
         <v>3392</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="28" t="s">
         <v>3393</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="28" t="s">
         <v>3394</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="28" t="s">
         <v>3395</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="28" t="s">
         <v>3397</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="28" t="s">
         <v>3398</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="28" t="s">
         <v>3399</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="22" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="28" t="s">
         <v>3401</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="28" t="s">
         <v>3402</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="28" t="s">
         <v>3394</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="28" t="s">
         <v>3395</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="28" t="s">
         <v>3397</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="28" t="s">
         <v>3398</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="28" t="s">
         <v>3403</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="22" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="28" t="s">
         <v>3404</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="28" t="s">
         <v>3405</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="28">
         <v>23</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="28" t="s">
         <v>3397</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28" t="s">
         <v>3406</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="28" t="s">
         <v>3407</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="22" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="28" t="s">
         <v>3408</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="28" t="s">
         <v>3409</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="28">
         <v>41</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="28" t="s">
         <v>3410</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35" t="s">
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="28" t="s">
         <v>3411</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="28" t="s">
         <v>3412</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="28" t="s">
         <v>868</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="28" t="s">
         <v>3398</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35" t="s">
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="28" t="s">
         <v>3413</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="28" t="s">
         <v>3414</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="28" t="s">
         <v>3415</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="28" t="s">
         <v>3398</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35" t="s">
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28" t="s">
         <v>3416</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="28" t="s">
         <v>3407</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="28" t="s">
         <v>3417</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="28" t="s">
         <v>3418</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="28" t="s">
         <v>478</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>3419</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="28" t="s">
         <v>3420</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="28" t="s">
         <v>3394</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="28" t="s">
         <v>3421</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="28" t="s">
         <v>3395</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="28" t="s">
         <v>3397</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35" t="s">
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="22" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="28" t="s">
         <v>3422</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="28" t="s">
         <v>3423</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="28" t="s">
         <v>3424</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="28" t="s">
         <v>3397</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35" t="s">
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28" t="s">
         <v>3425</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="28" t="s">
         <v>3407</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="28" t="s">
         <v>3426</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="28" t="s">
         <v>3427</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="28" t="s">
         <v>3428</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="28" t="s">
         <v>3397</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35" t="s">
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28" t="s">
         <v>3429</v>
       </c>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="28" t="s">
         <v>3430</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="28" t="s">
         <v>3431</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="28" t="s">
         <v>3394</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="28" t="s">
         <v>3421</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="28" t="s">
         <v>3395</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="28" t="s">
         <v>3396</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="28" t="s">
         <v>3397</v>
       </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35" t="s">
+      <c r="H12" s="28"/>
+      <c r="I12" s="28" t="s">
         <v>3432</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="28" t="s">
         <v>3400</v>
       </c>
     </row>
@@ -11683,8 +11622,8 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11697,1111 +11636,1111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="22" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="30" t="s">
         <v>3260</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="33" t="s">
         <v>3261</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="23"/>
       <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="27" t="s">
         <v>3262</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>3263</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="27" t="s">
         <v>3264</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="27" t="s">
         <v>3265</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="27" t="s">
         <v>3266</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="27" t="s">
         <v>3267</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="27" t="s">
         <v>3268</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="27" t="s">
         <v>3269</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F3" s="25"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="27" t="s">
         <v>3433</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="27" t="s">
         <v>3268</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="27" t="s">
         <v>3274</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="27" t="s">
         <v>3275</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="27" t="s">
         <v>3268</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="34" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="27" t="s">
         <v>3276</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="27" t="s">
         <v>3268</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="34" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="27" t="s">
         <v>3277</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="27" t="s">
         <v>3268</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="34" t="s">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="27" t="s">
         <v>3278</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="27" t="s">
         <v>3268</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="34" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="27" t="s">
         <v>3324</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="27" t="s">
         <v>3268</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="34" t="s">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="34" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="27" t="s">
         <v>3285</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="34" t="s">
+      <c r="D11" s="27"/>
+      <c r="E11" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="27" t="s">
         <v>3288</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="27" t="s">
         <v>3289</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="34" t="s">
+      <c r="D13" s="27"/>
+      <c r="E13" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="27" t="s">
         <v>3290</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="34" t="s">
+      <c r="D14" s="27"/>
+      <c r="E14" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="27" t="s">
         <v>3295</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="27" t="s">
         <v>3296</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="27" t="s">
         <v>3297</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="34" t="s">
+      <c r="D16" s="27"/>
+      <c r="E16" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="27" t="s">
         <v>3322</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="34" t="s">
+      <c r="D17" s="27"/>
+      <c r="E17" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="27" t="s">
         <v>3323</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="34" t="s">
+      <c r="D18" s="27"/>
+      <c r="E18" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="27" t="s">
         <v>3192</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="27" t="s">
         <v>3363</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="34" t="s">
+      <c r="D19" s="27"/>
+      <c r="E19" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="27" t="s">
         <v>3204</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="27" t="s">
         <v>3364</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="27" t="s">
         <v>3365</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F20" s="25"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="27" t="s">
         <v>3215</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="27" t="s">
         <v>3366</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="27" t="s">
         <v>3367</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="27" t="s">
         <v>3242</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="27" t="s">
         <v>3368</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="27" t="s">
         <v>3283</v>
       </c>
-      <c r="D22" s="41" t="s">
+      <c r="D22" s="27" t="s">
         <v>3369</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="27" t="s">
         <v>3332</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="27" t="s">
         <v>3333</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="27" t="s">
         <v>3334</v>
       </c>
-      <c r="D23" s="41" t="s">
-        <v>3434</v>
-      </c>
-      <c r="E23" s="34"/>
+      <c r="D23" s="27" t="s">
+        <v>3436</v>
+      </c>
+      <c r="E23" s="27"/>
       <c r="F23" s="25"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="27" t="s">
         <v>3335</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="27" t="s">
         <v>3336</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="27" t="s">
         <v>3334</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="27" t="s">
         <v>3337</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="E24" s="27"/>
       <c r="F24" s="25"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="27" t="s">
         <v>3338</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="27" t="s">
         <v>3339</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="27" t="s">
         <v>3334</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="27" t="s">
         <v>3340</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="E25" s="27"/>
       <c r="F25" s="25"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="27" t="s">
         <v>3341</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="27" t="s">
         <v>3342</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="27" t="s">
         <v>3334</v>
       </c>
-      <c r="D26" s="41" t="s">
+      <c r="D26" s="27" t="s">
         <v>3343</v>
       </c>
-      <c r="E26" s="34"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="25"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="27" t="s">
         <v>3347</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="27" t="s">
         <v>3348</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="27" t="s">
         <v>3334</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="27" t="s">
         <v>3349</v>
       </c>
-      <c r="E27" s="34"/>
+      <c r="E27" s="27"/>
       <c r="F27" s="25"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="32" t="s">
         <v>3352</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="32" t="s">
         <v>3353</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="32" t="s">
         <v>3334</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="D28" s="27" t="s">
         <v>3354</v>
       </c>
-      <c r="E28" s="34"/>
+      <c r="E28" s="27"/>
       <c r="F28" s="25"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="27" t="s">
         <v>3355</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="27" t="s">
         <v>3356</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="27" t="s">
         <v>3334</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="27" t="s">
         <v>3357</v>
       </c>
-      <c r="E29" s="34"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="25"/>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="27" t="s">
         <v>3300</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="27" t="s">
         <v>3301</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="27" t="s">
         <v>3302</v>
       </c>
-      <c r="D30" s="41" t="s">
-        <v>3436</v>
-      </c>
-      <c r="E30" s="34"/>
+      <c r="D30" s="27" t="s">
+        <v>3435</v>
+      </c>
+      <c r="E30" s="27"/>
       <c r="F30" s="25"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="27" t="s">
         <v>3303</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="27" t="s">
         <v>3304</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="27" t="s">
         <v>3302</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="27" t="s">
         <v>3305</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="25"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="27" t="s">
         <v>3306</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="27" t="s">
         <v>3307</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="27" t="s">
         <v>3302</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="27" t="s">
         <v>3308</v>
       </c>
-      <c r="E32" s="34"/>
+      <c r="E32" s="27"/>
       <c r="F32" s="25"/>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="27" t="s">
         <v>3309</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="27" t="s">
         <v>3310</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="27" t="s">
         <v>3302</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="27" t="s">
         <v>3311</v>
       </c>
-      <c r="E33" s="34"/>
+      <c r="E33" s="27"/>
       <c r="F33" s="25"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="27" t="s">
         <v>3312</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="27" t="s">
         <v>3313</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="27" t="s">
         <v>3302</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="27" t="s">
         <v>3314</v>
       </c>
-      <c r="E34" s="34"/>
+      <c r="E34" s="27"/>
       <c r="F34" s="25"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="27" t="s">
         <v>3315</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="27" t="s">
         <v>3316</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="27" t="s">
         <v>3302</v>
       </c>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="27" t="s">
         <v>3317</v>
       </c>
-      <c r="E35" s="34"/>
+      <c r="E35" s="27"/>
       <c r="F35" s="25"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="27" t="s">
         <v>3325</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="27" t="s">
         <v>3326</v>
       </c>
-      <c r="D36" s="41" t="s">
+      <c r="D36" s="27" t="s">
         <v>3327</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="27" t="s">
         <v>3328</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="27" t="s">
         <v>3326</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="34" t="s">
+      <c r="D37" s="27"/>
+      <c r="E37" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="31" t="s">
         <v>3374</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="27" t="s">
         <v>3375</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="27" t="s">
         <v>3376</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="34"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
       <c r="F38" s="25"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="31" t="s">
         <v>3377</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="27" t="s">
         <v>3378</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="27" t="s">
         <v>3376</v>
       </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="34"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
       <c r="F39" s="25"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="31" t="s">
         <v>3318</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="27" t="s">
         <v>3319</v>
       </c>
-      <c r="C40" s="34" t="s">
+      <c r="C40" s="27" t="s">
         <v>3320</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="27" t="s">
         <v>3321</v>
       </c>
-      <c r="E40" s="34"/>
+      <c r="E40" s="27"/>
       <c r="F40" s="25"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="27" t="s">
         <v>3291</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D41" s="41"/>
-      <c r="E41" s="34" t="s">
+      <c r="D41" s="27"/>
+      <c r="E41" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="27" t="s">
         <v>3293</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="34" t="s">
+      <c r="D42" s="27"/>
+      <c r="E42" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F42" s="25"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="27" t="s">
         <v>3294</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D43" s="41"/>
-      <c r="E43" s="34" t="s">
+      <c r="D43" s="27"/>
+      <c r="E43" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F43" s="25"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="27" t="s">
         <v>323</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="27" t="s">
         <v>3329</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D44" s="41" t="s">
+      <c r="D44" s="27" t="s">
         <v>3330</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B45" s="27" t="s">
         <v>3331</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D45" s="41"/>
-      <c r="E45" s="34" t="s">
+      <c r="D45" s="27"/>
+      <c r="E45" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="27" t="s">
         <v>3247</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="27" t="s">
         <v>3370</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="34" t="s">
+      <c r="D46" s="27"/>
+      <c r="E46" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="27" t="s">
         <v>3250</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="27" t="s">
         <v>3371</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D47" s="41" t="s">
+      <c r="D47" s="27" t="s">
         <v>3365</v>
       </c>
-      <c r="E47" s="34" t="s">
+      <c r="E47" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F47" s="25"/>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="27" t="s">
         <v>3252</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="27" t="s">
         <v>3366</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D48" s="41" t="s">
+      <c r="D48" s="27" t="s">
         <v>3367</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E48" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="27" t="s">
         <v>3254</v>
       </c>
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="27" t="s">
         <v>3372</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="27" t="s">
         <v>3292</v>
       </c>
-      <c r="D49" s="41" t="s">
+      <c r="D49" s="27" t="s">
         <v>3373</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="27" t="s">
         <v>3271</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="C50" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D50" s="41"/>
-      <c r="E50" s="34" t="s">
+      <c r="D50" s="27"/>
+      <c r="E50" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="27" t="s">
         <v>3273</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D51" s="41"/>
-      <c r="E51" s="34" t="s">
+      <c r="D51" s="27"/>
+      <c r="E51" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="27" t="s">
         <v>3279</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D52" s="41" t="s">
+      <c r="D52" s="27" t="s">
         <v>3280</v>
       </c>
-      <c r="E52" s="34" t="s">
+      <c r="E52" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F52" s="25"/>
       <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="27" t="s">
         <v>3281</v>
       </c>
-      <c r="C53" s="34" t="s">
+      <c r="C53" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D53" s="41" t="s">
+      <c r="D53" s="27" t="s">
         <v>3282</v>
       </c>
-      <c r="E53" s="34" t="s">
+      <c r="E53" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F53" s="25"/>
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="27" t="s">
         <v>3284</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="C54" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D54" s="41"/>
-      <c r="E54" s="34" t="s">
+      <c r="D54" s="27"/>
+      <c r="E54" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="27" t="s">
         <v>3286</v>
       </c>
-      <c r="C55" s="34" t="s">
+      <c r="C55" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D55" s="41" t="s">
+      <c r="D55" s="27" t="s">
         <v>3287</v>
       </c>
-      <c r="E55" s="34" t="s">
+      <c r="E55" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F55" s="26"/>
       <c r="G55" s="24"/>
     </row>
     <row r="56" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="27" t="s">
         <v>3298</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D56" s="41" t="s">
+      <c r="D56" s="27" t="s">
         <v>3299</v>
       </c>
-      <c r="E56" s="34" t="s">
+      <c r="E56" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F56" s="26"/>
       <c r="G56" s="24"/>
     </row>
     <row r="57" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="27" t="s">
         <v>3344</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="C57" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D57" s="41"/>
-      <c r="E57" s="34" t="s">
+      <c r="D57" s="27"/>
+      <c r="E57" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F57" s="24"/>
       <c r="G57" s="24"/>
     </row>
     <row r="58" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="B58" s="34" t="s">
+      <c r="B58" s="27" t="s">
         <v>3345</v>
       </c>
-      <c r="C58" s="34" t="s">
+      <c r="C58" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D58" s="41" t="s">
+      <c r="D58" s="27" t="s">
         <v>3346</v>
       </c>
-      <c r="E58" s="34" t="s">
+      <c r="E58" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="24"/>
     </row>
     <row r="59" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="34" t="s">
+      <c r="A59" s="27" t="s">
         <v>3145</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="27" t="s">
         <v>3350</v>
       </c>
-      <c r="C59" s="34" t="s">
+      <c r="C59" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D59" s="41"/>
-      <c r="E59" s="34" t="s">
+      <c r="D59" s="27"/>
+      <c r="E59" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F59" s="24"/>
       <c r="G59" s="24"/>
     </row>
     <row r="60" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="34" t="s">
+      <c r="A60" s="27" t="s">
         <v>3171</v>
       </c>
-      <c r="B60" s="34" t="s">
+      <c r="B60" s="27" t="s">
         <v>3351</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C60" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D60" s="41"/>
-      <c r="E60" s="34" t="s">
+      <c r="D60" s="27"/>
+      <c r="E60" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F60" s="24"/>
       <c r="G60" s="24"/>
     </row>
     <row r="61" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="34" t="s">
+      <c r="A61" s="27" t="s">
         <v>3358</v>
       </c>
-      <c r="B61" s="34" t="s">
+      <c r="B61" s="27" t="s">
         <v>3359</v>
       </c>
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D61" s="41" t="s">
+      <c r="D61" s="27" t="s">
         <v>3360</v>
       </c>
-      <c r="E61" s="34"/>
+      <c r="E61" s="27"/>
       <c r="F61" s="24"/>
       <c r="G61" s="24"/>
     </row>
     <row r="62" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="27" t="s">
         <v>3176</v>
       </c>
-      <c r="B62" s="34" t="s">
+      <c r="B62" s="27" t="s">
         <v>3361</v>
       </c>
-      <c r="C62" s="34" t="s">
+      <c r="C62" s="27" t="s">
         <v>3272</v>
       </c>
-      <c r="D62" s="41" t="s">
+      <c r="D62" s="27" t="s">
         <v>3362</v>
       </c>
-      <c r="E62" s="34" t="s">
+      <c r="E62" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F62" s="24"/>
       <c r="G62" s="24"/>
     </row>
     <row r="63" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="27" t="s">
         <v>3256</v>
       </c>
-      <c r="B63" s="34" t="s">
+      <c r="B63" s="27" t="s">
         <v>3379</v>
       </c>
-      <c r="C63" s="34" t="s">
+      <c r="C63" s="27" t="s">
         <v>3380</v>
       </c>
-      <c r="D63" s="41" t="s">
+      <c r="D63" s="27" t="s">
         <v>3381</v>
       </c>
-      <c r="E63" s="34" t="s">
+      <c r="E63" s="27" t="s">
         <v>3270</v>
       </c>
       <c r="F63" s="24"/>
       <c r="G63" s="24"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="36"/>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
@@ -12819,16 +12758,16 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C63">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"prescripteur"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"executant"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"prestation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"beneficiaire"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12847,8 +12786,8 @@
   </sheetPr>
   <dimension ref="A1:E2738"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A2164" workbookViewId="0">
+      <selection activeCell="B2184" sqref="B2184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12862,10 +12801,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
@@ -13122,7 +13061,7 @@
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>3435</v>
+        <v>3434</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>33</v>
@@ -34578,7 +34517,7 @@
       <c r="B2166" s="8" t="s">
         <v>3178</v>
       </c>
-      <c r="C2166" s="29" t="s">
+      <c r="C2166" s="38" t="s">
         <v>3179</v>
       </c>
     </row>
@@ -34589,7 +34528,7 @@
       <c r="B2167" s="8" t="s">
         <v>3180</v>
       </c>
-      <c r="C2167" s="30"/>
+      <c r="C2167" s="39"/>
       <c r="D2167" s="21"/>
       <c r="E2167" s="18"/>
     </row>
@@ -34600,7 +34539,7 @@
       <c r="B2168" s="8" t="s">
         <v>3181</v>
       </c>
-      <c r="C2168" s="31" t="s">
+      <c r="C2168" s="40" t="s">
         <v>3182</v>
       </c>
       <c r="D2168" s="21"/>
@@ -34613,7 +34552,7 @@
       <c r="B2169" s="8" t="s">
         <v>3183</v>
       </c>
-      <c r="C2169" s="32"/>
+      <c r="C2169" s="41"/>
       <c r="D2169" s="21"/>
       <c r="E2169" s="18"/>
     </row>
@@ -34624,7 +34563,7 @@
       <c r="B2170" s="8" t="s">
         <v>3184</v>
       </c>
-      <c r="C2170" s="32"/>
+      <c r="C2170" s="41"/>
       <c r="D2170" s="21"/>
       <c r="E2170" s="18"/>
     </row>
@@ -34635,7 +34574,7 @@
       <c r="B2171" s="8" t="s">
         <v>3185</v>
       </c>
-      <c r="C2171" s="32"/>
+      <c r="C2171" s="41"/>
       <c r="D2171" s="21"/>
       <c r="E2171" s="18"/>
     </row>
@@ -34646,7 +34585,7 @@
       <c r="B2172" s="8" t="s">
         <v>3186</v>
       </c>
-      <c r="C2172" s="32"/>
+      <c r="C2172" s="41"/>
       <c r="D2172" s="21"/>
       <c r="E2172" s="18"/>
     </row>
@@ -34657,7 +34596,7 @@
       <c r="B2173" s="8" t="s">
         <v>3187</v>
       </c>
-      <c r="C2173" s="32"/>
+      <c r="C2173" s="41"/>
       <c r="D2173" s="21"/>
       <c r="E2173" s="18"/>
     </row>
@@ -34668,7 +34607,7 @@
       <c r="B2174" s="8" t="s">
         <v>3188</v>
       </c>
-      <c r="C2174" s="32"/>
+      <c r="C2174" s="41"/>
       <c r="D2174" s="21"/>
       <c r="E2174" s="18"/>
     </row>
@@ -34679,7 +34618,7 @@
       <c r="B2175" s="8" t="s">
         <v>3189</v>
       </c>
-      <c r="C2175" s="32"/>
+      <c r="C2175" s="41"/>
       <c r="D2175" s="21"/>
       <c r="E2175" s="18"/>
     </row>
@@ -34690,7 +34629,7 @@
       <c r="B2176" s="8" t="s">
         <v>3190</v>
       </c>
-      <c r="C2176" s="32"/>
+      <c r="C2176" s="41"/>
       <c r="D2176" s="21"/>
       <c r="E2176" s="18"/>
     </row>
@@ -34701,7 +34640,7 @@
       <c r="B2177" s="8" t="s">
         <v>3191</v>
       </c>
-      <c r="C2177" s="33"/>
+      <c r="C2177" s="42"/>
       <c r="D2177" s="21"/>
       <c r="E2177" s="18"/>
     </row>
@@ -36160,5 +36099,6 @@
     <mergeCell ref="C2168:C2177"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>